<commit_message>
updated the pagebase removed getdriver method
</commit_message>
<xml_diff>
--- a/src/main/java/data/Testdata.xlsx
+++ b/src/main/java/data/Testdata.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Prod_TD" sheetId="1" r:id="rId1"/>
-    <sheet name="Locators" sheetId="2" r:id="rId2"/>
+    <sheet name="HomePageLocators" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>div.search-icon</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,9 +422,10 @@
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -443,8 +444,11 @@
       <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -463,15 +467,18 @@
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
@@ -489,7 +496,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final updates all Data Driven objects and values
</commit_message>
<xml_diff>
--- a/src/main/java/data/Testdata.xlsx
+++ b/src/main/java/data/Testdata.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Prod_TD" sheetId="1" r:id="rId1"/>
     <sheet name="HomePageLocators" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactPageLocators" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="SearchPageLocators" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>div.search-icon</t>
   </si>
@@ -70,6 +73,93 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>HomeContactLink</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>HomeConfirmBtn</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>HomeEmailField</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>HomeSubmitBtn</t>
+  </si>
+  <si>
+    <t>button.submit</t>
+  </si>
+  <si>
+    <t>HomeLanguageDropdown</t>
+  </si>
+  <si>
+    <t>select.locales-dropdown</t>
+  </si>
+  <si>
+    <t>div.nav-icon</t>
+  </si>
+  <si>
+    <t>HomeSideMenu</t>
+  </si>
+  <si>
+    <t>WEST</t>
+  </si>
+  <si>
+    <t>HomeMenuItem</t>
+  </si>
+  <si>
+    <t>input.input.search-input</t>
+  </si>
+  <si>
+    <t>SearchTextLocator</t>
+  </si>
+  <si>
+    <t>textarea.contact-msg</t>
+  </si>
+  <si>
+    <t>input.contact-input</t>
+  </si>
+  <si>
+    <t>ContactMessage</t>
+  </si>
+  <si>
+    <t>ContactFullName</t>
+  </si>
+  <si>
+    <t>contact-email</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>ContactConfirmCheckBox</t>
+  </si>
+  <si>
+    <t>button.contact-submit</t>
+  </si>
+  <si>
+    <t>ContactSubmitBtn</t>
+  </si>
+  <si>
+    <t>ContactSuccessMessage</t>
+  </si>
+  <si>
+    <t>p.feedback</t>
+  </si>
+  <si>
+    <t>MessageRegex</t>
+  </si>
+  <si>
+    <t>.*(Message|Successfully).*</t>
   </si>
 </sst>
 </file>
@@ -121,9 +211,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -409,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,64 +512,71 @@
     <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -493,34 +589,240 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>